<commit_message>
add tempalte relationship files
</commit_message>
<xml_diff>
--- a/output/frat/depth_1/embeddings/frat_updated_3_conceptnet_search_embeddings.xlsx
+++ b/output/frat/depth_1/embeddings/frat_updated_3_conceptnet_search_embeddings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\depth_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/depth_1/embeddings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876CD6C6-8C71-41DC-8B44-CC656A2731FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C765B-7D4E-274A-A90B-2F1FCD2135B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -646,19 +646,19 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="33.7265625" customWidth="1"/>
+    <col min="6" max="7" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -722,7 +722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -751,7 +751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -780,7 +780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -809,7 +809,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -867,7 +867,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -896,7 +896,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -925,7 +925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -954,7 +954,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -983,7 +983,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>

</xml_diff>